<commit_message>
add validation and remove some worksheet in employee profile import template
</commit_message>
<xml_diff>
--- a/templates/accupay-employeelist-template.xlsx
+++ b/templates/accupay-employeelist-template.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
-    <sheet name="Employee Dependents" sheetId="2" r:id="rId2"/>
-    <sheet name="Employee Salary" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Employee ID</t>
   </si>
@@ -85,21 +83,6 @@
   </si>
   <si>
     <t>Marital Status(Single/Married/N/A)</t>
-  </si>
-  <si>
-    <t>Relationship to Employee</t>
-  </si>
-  <si>
-    <t>Basic pay</t>
-  </si>
-  <si>
-    <t>Effective date from</t>
-  </si>
-  <si>
-    <t>Effective date to</t>
-  </si>
-  <si>
-    <t>Undeclared</t>
   </si>
   <si>
     <t>Works days per year</t>
@@ -152,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
@@ -180,20 +163,14 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="0"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -594,147 +571,26 @@
       <c r="W1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>28</v>
+      <c r="X1" s="14" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection insertRows="0" deleteRows="0" selectLockedCells="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Q1"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="20" style="4" customWidth="1"/>
-    <col min="15" max="15" width="20.140625" style="5" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" style="6" customWidth="1"/>
-    <col min="17" max="17" width="19" style="6" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="P1" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="C841" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr codeName="Sheet3"/>
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="22.140625" style="1" customWidth="1"/>
-    <col min="2" max="3" width="22.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <sheetProtection password="C841" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" selectLockedCells="1"/>
+  <sheetProtection password="CD03" sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+      <formula1>"Male,Female"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
+      <formula1>"Single,Married"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S1:S1048576">
+      <formula1>"WEEKLY,SEMI-MONTHLY"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T1:T1048576">
+      <formula1>"Daily,Monthly"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>